<commit_message>
reupload unit status as issued and script to delete projects
</commit_message>
<xml_diff>
--- a/output/Uncleaned_CDM_Projects.xlsx
+++ b/output/Uncleaned_CDM_Projects.xlsx
@@ -211,87 +211,87 @@
     <t>Reporting date</t>
   </si>
   <si>
+    <t>0SERXDY1GS89I4BD3T8QL8NPI6Z34A/</t>
+  </si>
+  <si>
+    <t>Aux_ACG70V0UUUPNDPCRJL8KRYLHHSB0CJ</t>
+  </si>
+  <si>
+    <t>D8IRSCM3W0ZGKAFXYJOQVL6HP2NEBU</t>
+  </si>
+  <si>
+    <t>UBX0FC1NMA8IV9H5LTOEG3PJKZSWD6</t>
+  </si>
+  <si>
+    <t>DB/Z31DKITEOQXOLO3V5IMYVBGQ8IYZP4</t>
+  </si>
+  <si>
+    <t>LGABR9Q0JYH68VN5WI7MUXTEKDCSOP</t>
+  </si>
+  <si>
+    <t>A39MS6G57IZHWTBEVNPXRJOFL8K01C</t>
+  </si>
+  <si>
     <t>Idval</t>
   </si>
   <si>
+    <t>EL9SWD7R6H4MKP3CB8XUYAOFN2J5TZ</t>
+  </si>
+  <si>
     <t>BDF248C6JG1SKOZYQ5T3WVEHR7MXLU</t>
   </si>
   <si>
-    <t>0SERXDY1GS89I4BD3T8QL8NPI6Z34A/</t>
-  </si>
-  <si>
-    <t>A39MS6G57IZHWTBEVNPXRJOFL8K01C</t>
-  </si>
-  <si>
-    <t>DB/Z31DKITEOQXOLO3V5IMYVBGQ8IYZP4</t>
-  </si>
-  <si>
-    <t>Aux_ACG70V0UUUPNDPCRJL8KRYLHHSB0CJ</t>
-  </si>
-  <si>
-    <t>UBX0FC1NMA8IV9H5LTOEG3PJKZSWD6</t>
-  </si>
-  <si>
-    <t>D8IRSCM3W0ZGKAFXYJOQVL6HP2NEBU</t>
-  </si>
-  <si>
-    <t>EL9SWD7R6H4MKP3CB8XUYAOFN2J5TZ</t>
-  </si>
-  <si>
-    <t>LGABR9Q0JYH68VN5WI7MUXTEKDCSOP</t>
-  </si>
-  <si>
     <t>PA</t>
   </si>
   <si>
     <t>PoA</t>
   </si>
   <si>
+    <t>Landfill gas</t>
+  </si>
+  <si>
+    <t>Methane avoidance</t>
+  </si>
+  <si>
+    <t>EE households</t>
+  </si>
+  <si>
+    <t>EE Industry</t>
+  </si>
+  <si>
+    <t>Waste</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
     <t>Solar</t>
   </si>
   <si>
-    <t>Methane avoidance</t>
-  </si>
-  <si>
-    <t>Landfill gas</t>
-  </si>
-  <si>
-    <t>Transport</t>
-  </si>
-  <si>
-    <t>Waste</t>
-  </si>
-  <si>
-    <t>EE Industry</t>
-  </si>
-  <si>
-    <t>EE households</t>
-  </si>
-  <si>
     <t>Mixed renewables</t>
   </si>
   <si>
+    <t>Landfill flaring</t>
+  </si>
+  <si>
+    <t>Domestic manure</t>
+  </si>
+  <si>
+    <t>Stoves</t>
+  </si>
+  <si>
+    <t>Building materials</t>
+  </si>
+  <si>
+    <t>Waste water</t>
+  </si>
+  <si>
+    <t>Mode shift: road to rail</t>
+  </si>
+  <si>
     <t>Solar PV</t>
   </si>
   <si>
-    <t>Waste water</t>
-  </si>
-  <si>
-    <t>Landfill flaring</t>
-  </si>
-  <si>
-    <t>Mode shift: road to rail</t>
-  </si>
-  <si>
-    <t>Domestic manure</t>
-  </si>
-  <si>
-    <t>Building materials</t>
-  </si>
-  <si>
-    <t>Stoves</t>
-  </si>
-  <si>
     <t>Solar &amp; wind</t>
   </si>
   <si>
@@ -310,7 +310,7 @@
     <t>2023m8</t>
   </si>
   <si>
-    <t>03Nov2023</t>
+    <t>10Oct2024</t>
   </si>
 </sst>
 </file>
@@ -902,7 +902,7 @@
     </row>
     <row r="3" spans="1:66">
       <c r="A3" s="1">
-        <v>8860</v>
+        <v>8841</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -946,7 +946,7 @@
     </row>
     <row r="4" spans="1:66">
       <c r="A4" s="1">
-        <v>9218</v>
+        <v>9035</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -990,7 +990,7 @@
     </row>
     <row r="5" spans="1:66">
       <c r="A5" s="1">
-        <v>9434</v>
+        <v>9477</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="6" spans="1:66">
       <c r="A6" s="1">
-        <v>9479</v>
+        <v>10034</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="7" spans="1:66">
       <c r="A7" s="1">
-        <v>10170</v>
+        <v>10123</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1093,7 +1093,7 @@
         <v>81</v>
       </c>
       <c r="J7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="8" spans="1:66">
       <c r="A8" s="1">
-        <v>10272</v>
+        <v>10532</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1134,10 +1134,10 @@
         <v>76</v>
       </c>
       <c r="I8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -1166,7 +1166,7 @@
     </row>
     <row r="9" spans="1:66">
       <c r="A9" s="1">
-        <v>10404</v>
+        <v>10965</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1210,7 +1210,7 @@
     </row>
     <row r="10" spans="1:66">
       <c r="A10" s="1">
-        <v>11243</v>
+        <v>11363</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1254,7 +1254,7 @@
     </row>
     <row r="11" spans="1:66">
       <c r="A11" s="1">
-        <v>11518</v>
+        <v>11698</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="12" spans="1:66">
       <c r="A12" s="1">
-        <v>13073</v>
+        <v>11745</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1310,10 +1310,10 @@
         <v>76</v>
       </c>
       <c r="I12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="V12">
         <v>0</v>

</xml_diff>